<commit_message>
Lots of plotting work. Altso the beginning of doing test/training splits
</commit_message>
<xml_diff>
--- a/plots/medians_per_subcel_location.xlsx
+++ b/plots/medians_per_subcel_location.xlsx
@@ -669,7 +669,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>153.7963772045516</v>
+        <v>2.982993458012097</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -680,7 +680,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>150.5706554465452</v>
+        <v>3.185281877226719</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -691,7 +691,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>11.65850626862809</v>
+        <v>0.5000899561570841</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -702,7 +702,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>8.028519664935775</v>
+        <v>0.2356382498269848</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -713,7 +713,7 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>3.097318912591089</v>
+        <v>0.1248707319547105</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -724,7 +724,7 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>97.1782768104508</v>
+        <v>1.804617069099212</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -735,7 +735,7 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>42.95628325304153</v>
+        <v>0.9854420787266219</v>
       </c>
       <c r="C8">
         <v>47</v>
@@ -746,7 +746,7 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>30.29466516097704</v>
+        <v>0.7234265434288588</v>
       </c>
       <c r="C9">
         <v>27</v>
@@ -757,7 +757,7 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>97.1782768104508</v>
+        <v>1.804617069099212</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -768,7 +768,7 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>40.98879467878215</v>
+        <v>0.8387175341099418</v>
       </c>
       <c r="C11">
         <v>4</v>
@@ -779,7 +779,7 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>22.73287418603913</v>
+        <v>0.4528785591104308</v>
       </c>
       <c r="C12">
         <v>6</v>
@@ -790,7 +790,7 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>35.03684859388605</v>
+        <v>0.8252109522374417</v>
       </c>
       <c r="C13">
         <v>28</v>
@@ -801,7 +801,7 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>28.80434909471444</v>
+        <v>0.5730396440149269</v>
       </c>
       <c r="C14">
         <v>10</v>
@@ -812,7 +812,7 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>76.713232971392</v>
+        <v>1.374095329832081</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -823,7 +823,7 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>97.19156473961337</v>
+        <v>1.684025186837135</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -834,7 +834,7 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>53.52395478410785</v>
+        <v>1.072034271432329</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -845,7 +845,7 @@
         <v>19</v>
       </c>
       <c r="B18">
-        <v>35.56255746960407</v>
+        <v>0.6806268500810692</v>
       </c>
       <c r="C18">
         <v>3</v>
@@ -856,7 +856,7 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>54.75234974884314</v>
+        <v>1.06643168202768</v>
       </c>
       <c r="C19">
         <v>171</v>
@@ -867,7 +867,7 @@
         <v>21</v>
       </c>
       <c r="B20">
-        <v>98.01354954925432</v>
+        <v>1.759134974917344</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -878,7 +878,7 @@
         <v>22</v>
       </c>
       <c r="B21">
-        <v>80.29955153606861</v>
+        <v>1.405857137272286</v>
       </c>
       <c r="C21">
         <v>13</v>
@@ -889,7 +889,7 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>44.18488722123552</v>
+        <v>0.9140008136579252</v>
       </c>
       <c r="C22">
         <v>56</v>
@@ -900,7 +900,7 @@
         <v>24</v>
       </c>
       <c r="B23">
-        <v>78.98631593932105</v>
+        <v>1.415993033268747</v>
       </c>
       <c r="C23">
         <v>4</v>
@@ -911,7 +911,7 @@
         <v>25</v>
       </c>
       <c r="B24">
-        <v>54.43450274253281</v>
+        <v>0.9968082181388143</v>
       </c>
       <c r="C24">
         <v>7</v>
@@ -922,7 +922,7 @@
         <v>26</v>
       </c>
       <c r="B25">
-        <v>2.41523278793059</v>
+        <v>0.09864551507746874</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -933,7 +933,7 @@
         <v>27</v>
       </c>
       <c r="B26">
-        <v>89.07121778088256</v>
+        <v>1.55494819431765</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -944,7 +944,7 @@
         <v>28</v>
       </c>
       <c r="B27">
-        <v>41.33078948226365</v>
+        <v>0.6974394253448498</v>
       </c>
       <c r="C27">
         <v>3</v>
@@ -955,7 +955,7 @@
         <v>29</v>
       </c>
       <c r="B28">
-        <v>97.50724792388603</v>
+        <v>1.858052519626876</v>
       </c>
       <c r="C28">
         <v>3</v>
@@ -966,7 +966,7 @@
         <v>30</v>
       </c>
       <c r="B29">
-        <v>66.63017114333371</v>
+        <v>1.131880927038853</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -977,7 +977,7 @@
         <v>31</v>
       </c>
       <c r="B30">
-        <v>42.68506996366664</v>
+        <v>0.8843010928965391</v>
       </c>
       <c r="C30">
         <v>6</v>
@@ -988,7 +988,7 @@
         <v>32</v>
       </c>
       <c r="B31">
-        <v>12.65476818720824</v>
+        <v>0.5771152653830183</v>
       </c>
       <c r="C31">
         <v>5</v>
@@ -999,7 +999,7 @@
         <v>33</v>
       </c>
       <c r="B32">
-        <v>12.65476818720824</v>
+        <v>0.5771152653830183</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1010,7 +1010,7 @@
         <v>34</v>
       </c>
       <c r="B33">
-        <v>24.56441796546291</v>
+        <v>0.6399297951078362</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -1021,7 +1021,7 @@
         <v>35</v>
       </c>
       <c r="B34">
-        <v>23.6135367267666</v>
+        <v>0.537443682613347</v>
       </c>
       <c r="C34">
         <v>7</v>
@@ -1032,7 +1032,7 @@
         <v>36</v>
       </c>
       <c r="B35">
-        <v>11.65850626862809</v>
+        <v>0.5000899561570841</v>
       </c>
       <c r="C35">
         <v>3</v>
@@ -1043,7 +1043,7 @@
         <v>37</v>
       </c>
       <c r="B36">
-        <v>7.639356521232168</v>
+        <v>0.3485095648908511</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1054,7 +1054,7 @@
         <v>38</v>
       </c>
       <c r="B37">
-        <v>6.894072589104854</v>
+        <v>0.2134279081879926</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -1065,7 +1065,7 @@
         <v>39</v>
       </c>
       <c r="B38">
-        <v>16.29460950732074</v>
+        <v>0.4528785591104308</v>
       </c>
       <c r="C38">
         <v>4</v>
@@ -1076,7 +1076,7 @@
         <v>40</v>
       </c>
       <c r="B39">
-        <v>66.66073180859341</v>
+        <v>1.33563522521528</v>
       </c>
       <c r="C39">
         <v>6</v>
@@ -1087,7 +1087,7 @@
         <v>41</v>
       </c>
       <c r="B40">
-        <v>14.9424648224781</v>
+        <v>0.489449455794709</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -1098,7 +1098,7 @@
         <v>42</v>
       </c>
       <c r="B41">
-        <v>35.26281630484193</v>
+        <v>0.8429960974594664</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -1109,7 +1109,7 @@
         <v>43</v>
       </c>
       <c r="B42">
-        <v>46.16715410956121</v>
+        <v>0.8264765188794441</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -1120,7 +1120,7 @@
         <v>44</v>
       </c>
       <c r="B43">
-        <v>13.3004855455531</v>
+        <v>0.4947697059758965</v>
       </c>
       <c r="C43">
         <v>2</v>
@@ -1131,7 +1131,7 @@
         <v>45</v>
       </c>
       <c r="B44">
-        <v>18.54789339654436</v>
+        <v>0.3563042493206986</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -1142,7 +1142,7 @@
         <v>46</v>
       </c>
       <c r="B45">
-        <v>57.51791019883576</v>
+        <v>1.095018225019914</v>
       </c>
       <c r="C45">
         <v>9</v>
@@ -1153,7 +1153,7 @@
         <v>47</v>
       </c>
       <c r="B46">
-        <v>97.1782768104508</v>
+        <v>1.804617069099212</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -1164,7 +1164,7 @@
         <v>48</v>
       </c>
       <c r="B47">
-        <v>72.07220546954159</v>
+        <v>1.730106732928166</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -1175,7 +1175,7 @@
         <v>49</v>
       </c>
       <c r="B48">
-        <v>40.36338051004815</v>
+        <v>0.9104918665247099</v>
       </c>
       <c r="C48">
         <v>30</v>
@@ -1186,7 +1186,7 @@
         <v>50</v>
       </c>
       <c r="B49">
-        <v>43.624374873345</v>
+        <v>0.8459799601421594</v>
       </c>
       <c r="C49">
         <v>4</v>
@@ -1197,7 +1197,7 @@
         <v>51</v>
       </c>
       <c r="B50">
-        <v>18.83545796459087</v>
+        <v>0.5413315018234505</v>
       </c>
       <c r="C50">
         <v>3</v>
@@ -1208,7 +1208,7 @@
         <v>52</v>
       </c>
       <c r="B51">
-        <v>42.83884932967503</v>
+        <v>0.7234265434288588</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -1219,7 +1219,7 @@
         <v>53</v>
       </c>
       <c r="B52">
-        <v>42.83884932967503</v>
+        <v>0.7234265434288588</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -1230,7 +1230,7 @@
         <v>54</v>
       </c>
       <c r="B53">
-        <v>74.63279307232359</v>
+        <v>1.403978974286529</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -1241,7 +1241,7 @@
         <v>55</v>
       </c>
       <c r="B54">
-        <v>83.96938513633744</v>
+        <v>1.845312545345013</v>
       </c>
       <c r="C54">
         <v>2</v>
@@ -1252,7 +1252,7 @@
         <v>56</v>
       </c>
       <c r="B55">
-        <v>77.44828588020209</v>
+        <v>1.375318573454345</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -1263,7 +1263,7 @@
         <v>57</v>
       </c>
       <c r="B56">
-        <v>35.12892102853821</v>
+        <v>0.7928173930677473</v>
       </c>
       <c r="C56">
         <v>6</v>
@@ -1274,7 +1274,7 @@
         <v>58</v>
       </c>
       <c r="B57">
-        <v>72.07220546954159</v>
+        <v>1.730106732928166</v>
       </c>
       <c r="C57">
         <v>3</v>
@@ -1285,7 +1285,7 @@
         <v>59</v>
       </c>
       <c r="B58">
-        <v>51.75568838810951</v>
+        <v>1.069346497970898</v>
       </c>
       <c r="C58">
         <v>94</v>
@@ -1296,7 +1296,7 @@
         <v>60</v>
       </c>
       <c r="B59">
-        <v>74.63279307232359</v>
+        <v>1.403978974286529</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -1307,7 +1307,7 @@
         <v>61</v>
       </c>
       <c r="B60">
-        <v>72.07220546954159</v>
+        <v>1.730106732928166</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -1318,7 +1318,7 @@
         <v>62</v>
       </c>
       <c r="B61">
-        <v>16.07103727692233</v>
+        <v>0.6264547007678573</v>
       </c>
       <c r="C61">
         <v>2</v>
@@ -1329,7 +1329,7 @@
         <v>63</v>
       </c>
       <c r="B62">
-        <v>156.2802640040468</v>
+        <v>3.190535134532942</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -1340,7 +1340,7 @@
         <v>64</v>
       </c>
       <c r="B63">
-        <v>55.92561874816832</v>
+        <v>1.299446308105855</v>
       </c>
       <c r="C63">
         <v>8</v>
@@ -1351,7 +1351,7 @@
         <v>65</v>
       </c>
       <c r="B64">
-        <v>9.648931394930131</v>
+        <v>0.4242997605239676</v>
       </c>
       <c r="C64">
         <v>2</v>
@@ -1362,7 +1362,7 @@
         <v>66</v>
       </c>
       <c r="B65">
-        <v>97.50724792388603</v>
+        <v>1.858052519626876</v>
       </c>
       <c r="C65">
         <v>9</v>
@@ -1373,7 +1373,7 @@
         <v>67</v>
       </c>
       <c r="B66">
-        <v>57.51791019883576</v>
+        <v>1.095018225019914</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -1384,7 +1384,7 @@
         <v>68</v>
       </c>
       <c r="B67">
-        <v>20.80453969382964</v>
+        <v>0.5220658354212935</v>
       </c>
       <c r="C67">
         <v>3</v>
@@ -1395,7 +1395,7 @@
         <v>69</v>
       </c>
       <c r="B68">
-        <v>5.344964592424926</v>
+        <v>0.1998367827839339</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -1406,7 +1406,7 @@
         <v>70</v>
       </c>
       <c r="B69">
-        <v>108.4461431375644</v>
+        <v>1.900160076847982</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -1417,7 +1417,7 @@
         <v>71</v>
       </c>
       <c r="B70">
-        <v>5.027294654581379</v>
+        <v>0.2235775399841599</v>
       </c>
       <c r="C70">
         <v>2</v>
@@ -1428,7 +1428,7 @@
         <v>72</v>
       </c>
       <c r="B71">
-        <v>5.344964592424926</v>
+        <v>0.1998367827839339</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -1439,7 +1439,7 @@
         <v>73</v>
       </c>
       <c r="B72">
-        <v>80.29955153606861</v>
+        <v>1.573281009989405</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -1450,7 +1450,7 @@
         <v>74</v>
       </c>
       <c r="B73">
-        <v>102.8261629470646</v>
+        <v>1.812666695838897</v>
       </c>
       <c r="C73">
         <v>2</v>
@@ -1461,7 +1461,7 @@
         <v>75</v>
       </c>
       <c r="B74">
-        <v>14.9424648224781</v>
+        <v>0.489449455794709</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -1472,7 +1472,7 @@
         <v>76</v>
       </c>
       <c r="B75">
-        <v>19.16159241295641</v>
+        <v>0.5086371355091618</v>
       </c>
       <c r="C75">
         <v>2</v>
@@ -1483,7 +1483,7 @@
         <v>77</v>
       </c>
       <c r="B76">
-        <v>24.86646095938994</v>
+        <v>0.4684272258084257</v>
       </c>
       <c r="C76">
         <v>2</v>
@@ -1494,7 +1494,7 @@
         <v>78</v>
       </c>
       <c r="B77">
-        <v>31.59828101922354</v>
+        <v>0.5674970173644726</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -1505,7 +1505,7 @@
         <v>79</v>
       </c>
       <c r="B78">
-        <v>58.07996957879475</v>
+        <v>1.030943476651703</v>
       </c>
       <c r="C78">
         <v>4</v>
@@ -1516,7 +1516,7 @@
         <v>80</v>
       </c>
       <c r="B79">
-        <v>98.53912752532145</v>
+        <v>2.063481559231944</v>
       </c>
       <c r="C79">
         <v>6</v>
@@ -1527,7 +1527,7 @@
         <v>81</v>
       </c>
       <c r="B80">
-        <v>7.606341734319243</v>
+        <v>0.3591002507456232</v>
       </c>
       <c r="C80">
         <v>6</v>
@@ -1538,7 +1538,7 @@
         <v>82</v>
       </c>
       <c r="B81">
-        <v>48.48659441674303</v>
+        <v>0.9848190030180373</v>
       </c>
       <c r="C81">
         <v>4</v>
@@ -1549,7 +1549,7 @@
         <v>83</v>
       </c>
       <c r="B82">
-        <v>51.68619227708592</v>
+        <v>1.019558080821817</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -1560,7 +1560,7 @@
         <v>84</v>
       </c>
       <c r="B83">
-        <v>17.46683275901559</v>
+        <v>0.5220658354212935</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -1571,7 +1571,7 @@
         <v>85</v>
       </c>
       <c r="B84">
-        <v>9.142595114121329</v>
+        <v>0.303333355177287</v>
       </c>
       <c r="C84">
         <v>6</v>
@@ -1582,7 +1582,7 @@
         <v>86</v>
       </c>
       <c r="B85">
-        <v>80.29955153606861</v>
+        <v>1.573281009989405</v>
       </c>
       <c r="C85">
         <v>1</v>
@@ -1593,7 +1593,7 @@
         <v>87</v>
       </c>
       <c r="B86">
-        <v>11.65850626862809</v>
+        <v>0.5000899561570841</v>
       </c>
       <c r="C86">
         <v>1</v>
@@ -1604,7 +1604,7 @@
         <v>88</v>
       </c>
       <c r="B87">
-        <v>61.06752107730522</v>
+        <v>1.405919626969103</v>
       </c>
       <c r="C87">
         <v>2</v>
@@ -1615,7 +1615,7 @@
         <v>89</v>
       </c>
       <c r="B88">
-        <v>99.2580392126074</v>
+        <v>1.954409497046345</v>
       </c>
       <c r="C88">
         <v>2</v>
@@ -1626,7 +1626,7 @@
         <v>90</v>
       </c>
       <c r="B89">
-        <v>31.42797766032423</v>
+        <v>0.7614428806699844</v>
       </c>
       <c r="C89">
         <v>2</v>
@@ -1637,7 +1637,7 @@
         <v>91</v>
       </c>
       <c r="B90">
-        <v>19.79169709778491</v>
+        <v>0.3999049564437642</v>
       </c>
       <c r="C90">
         <v>1</v>

</xml_diff>